<commit_message>
use Japanse in sheet label.
</commit_message>
<xml_diff>
--- a/test/fixtures/excel/2007_ja.xlsx
+++ b/test/fixtures/excel/2007_ja.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="692" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="686" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="シート1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="シート2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -71,6 +71,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -139,15 +140,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.321568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.3843137254902"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -155,7 +156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -163,7 +164,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
@@ -189,15 +190,15 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.321568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.3843137254902"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -205,7 +206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -236,7 +237,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.321568627451"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="0" width="10.3843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>